<commit_message>
ar4 done Titanic to reformat2
</commit_message>
<xml_diff>
--- a/Reports/day4/tp4_1.xlsx
+++ b/Reports/day4/tp4_1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Title</t>
   </si>
@@ -184,8 +184,10 @@
     <t>We would like to extract from our list all the surnames and first names of the Ladies and copy them elsewhere on the sheet.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Retour blended :: =BDMOYENNE or = DAVERAGE(A4:D8, "Unit Cost", A1:B2)
-=BDMOYENNE(A4:D8, 3, A1:B2) or =DAVERAGE</t>
+    <t>BDMOYENNE</t>
+  </si>
+  <si>
+    <t>DAVERAGE</t>
   </si>
 </sst>
 </file>
@@ -542,7 +544,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,8 +840,16 @@
       <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="7"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>